<commit_message>
Start working on Class 4
</commit_message>
<xml_diff>
--- a/Class3/t-tests and ANOVA with Excel_new.xlsx
+++ b/Class3/t-tests and ANOVA with Excel_new.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>BU</t>
   </si>
@@ -59,6 +59,27 @@
   </si>
   <si>
     <t>p(Welch)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>eta-squared</t>
   </si>
 </sst>
 </file>
@@ -125,7 +146,27 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1203,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1215,7 +1256,7 @@
     <col min="2" max="3" width="13.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1226,269 +1267,338 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <f ca="1">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>110.77424372452056</v>
+        <v>109.39488671604914</v>
       </c>
       <c r="B2">
         <f ca="1">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>64.47244669343948</v>
+        <v>111.69076324697491</v>
       </c>
       <c r="C2">
         <f ca="1">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>97.436028872023968</v>
+        <v>115.41871803302236</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f t="shared" ref="A3:C11" ca="1" si="0">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>111.18277494508111</v>
+        <v>79.069454564139718</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>104.00851710087687</v>
+        <v>93.61365160540791</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>113.44632888981609</v>
+        <v>105.53439856253917</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <f ca="1">(A12-B12)/SQRT((A13^2/10)+(B13^2/10))</f>
+        <v>3.3913109062065162E-2</v>
+      </c>
+      <c r="G3">
+        <f ca="1">(B12-C12)/SQRT((B13^2/10)+(C13^2/10))</f>
+        <v>1.7368849307001935</v>
+      </c>
+      <c r="H3">
+        <f ca="1">(A12-C12)/SQRT((A13^2/10)+(C13^2/10))</f>
+        <v>1.9496982525078208</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>99.510744970934581</v>
+        <v>108.86749043435451</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>114.35597027249754</v>
+        <v>92.109101633576842</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>112.31047154767127</v>
+        <v>89.658430759670708</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>115.64627328444787</v>
+        <v>103.44517528718657</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>106.26060859338915</v>
+        <v>103.63523323772927</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>81.848978318020457</v>
+        <v>90.34024033741899</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <f ca="1">_xlfn.T.DIST.2T(ABS(F3), F4)</f>
+        <v>0.97331968033560579</v>
+      </c>
+      <c r="G5" s="2">
+        <f ca="1">_xlfn.T.DIST.2T(ABS(G3), G4)</f>
+        <v>9.9489449814553155E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <f ca="1">_xlfn.T.DIST.2T(ABS(H3), H4)</f>
+        <v>6.6965694806031276E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>93.743268911327974</v>
+        <v>101.63413004660282</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>99.168848902691735</v>
+        <v>92.579288610768657</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>102.96013634122684</v>
+        <v>85.739435367981116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <f ca="1">_xlfn.T.TEST(A2:A11,B2:B11,2,2)</f>
+        <v>0.97331968033559724</v>
+      </c>
+      <c r="G6">
+        <f ca="1">_xlfn.T.TEST(B2:B11,C2:C11,2,2)</f>
+        <v>9.948944981455568E-2</v>
+      </c>
+      <c r="H6">
+        <f ca="1">_xlfn.T.TEST(A2:A11,C2:C11,2,2)</f>
+        <v>6.6965694806032899E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>122.49711533767726</v>
+        <v>99.268983966636654</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>106.98483718017883</v>
+        <v>82.628191960013424</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>104.31522277096495</v>
+        <v>70.805998667596796</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <f ca="1">_xlfn.T.TEST(A2:A11,B2:B11,2,3)</f>
+        <v>0.9733367261729714</v>
+      </c>
+      <c r="G7">
+        <f ca="1">_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
+        <v>9.9490283546276301E-2</v>
+      </c>
+      <c r="H7">
+        <f ca="1">_xlfn.T.TEST(A2:A11,C2:C11,2,3)</f>
+        <v>6.7655214580088718E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>100.7626921683558</v>
+        <v>109.13479561612924</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>91.065613813359278</v>
+        <v>88.841247912796305</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>115.84262669682269</v>
+        <v>100.94901760863864</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>83.040724557222944</v>
+        <v>91.051750468180856</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>96.787238102175678</v>
+        <v>125.1169401173814</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>122.63809065265588</v>
+        <v>63.223695712253026</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>116.71588493554404</v>
+        <v>125.65368661772681</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>83.664210254002754</v>
+        <v>103.10255781695592</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>91.229012621385891</v>
+        <v>93.025407921119168</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>94.599837489824068</v>
+        <v>96.724414923420682</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>90.779303261639825</v>
+        <v>128.79822949334647</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96.004106431789666</v>
+        <v>87.636465797908372</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f ca="1">AVERAGE(A2:A11)</f>
-        <v>104.84735603249362</v>
+        <v>102.4244768640427</v>
       </c>
       <c r="B12">
         <f ca="1">AVERAGE(B2:B11)</f>
-        <v>95.75475941742512</v>
+        <v>102.21152056349513</v>
       </c>
       <c r="C12">
         <f ca="1">AVERAGE(C2:C11)</f>
-        <v>103.80310031423778</v>
+        <v>90.233180876814842</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f ca="1">_xlfn.STDEV.S(A2:A11)</f>
-        <v>12.442148733953134</v>
+        <v>12.443802063351592</v>
       </c>
       <c r="B13">
         <f ca="1">_xlfn.STDEV.S(B2:B11)</f>
-        <v>14.27837063834702</v>
+        <v>15.474787181704411</v>
       </c>
       <c r="C13">
         <f ca="1">_xlfn.STDEV.S(C2:C11)</f>
-        <v>12.5055640734703</v>
+        <v>15.366885059951855</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <f ca="1">(A12-B12)/SQRT((A13^2/10)+(B13^2/10))</f>
-        <v>1.5182209840851779</v>
-      </c>
-      <c r="C16">
-        <f ca="1">(B12-C12)/SQRT((B13^2/10)+(C13^2/10))</f>
-        <v>-1.3409041581397032</v>
-      </c>
-      <c r="D16">
-        <f ca="1">(A12-C12)/SQRT((A13^2/10)+(C13^2/10))</f>
-        <v>0.18719305021614827</v>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <f ca="1">10*((A12-AVERAGE(A2:C11))^2+(B12-AVERAGE(A2:C11))^2+(C12-AVERAGE(A2:C11))^2)</f>
+        <v>973.84556627880329</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f ca="1">B17/C17</f>
+        <v>486.92278313940164</v>
+      </c>
+      <c r="E17">
+        <f ca="1">D17/D18</f>
+        <v>2.3169940139751697</v>
+      </c>
+      <c r="F17">
+        <f ca="1">_xlfn.F.DIST.RT(E17,2,27)</f>
+        <v>0.11785080303218637</v>
+      </c>
+      <c r="G17">
+        <f ca="1">B17/B19</f>
+        <v>0.14648763298057649</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>18</v>
-      </c>
-      <c r="C17">
-        <v>18</v>
-      </c>
-      <c r="D17">
-        <v>18</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <f ca="1">DEVSQ(A2:A11)+DEVSQ(B2:B11)+DEVSQ(C2:C11)</f>
+        <v>5674.1256410102815</v>
+      </c>
+      <c r="C18">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:D19" ca="1" si="1">B18/C18</f>
+        <v>210.15280151889931</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2">
-        <f ca="1">_xlfn.T.DIST.2T(ABS(B16), B17)</f>
-        <v>0.14632706712264132</v>
-      </c>
-      <c r="C18" s="2">
-        <f ca="1">_xlfn.T.DIST.2T(ABS(C16), C17)</f>
-        <v>0.19662896811676292</v>
-      </c>
-      <c r="D18" s="2">
-        <f ca="1">_xlfn.T.DIST.2T(ABS(D16), D17)</f>
-        <v>0.85360310270469764</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B19">
-        <f ca="1">_xlfn.T.TEST(A2:A11,B2:B11,2,2)</f>
-        <v>0.14632706712264199</v>
+        <f ca="1">DEVSQ(A2:C11)</f>
+        <v>6647.9712072890843</v>
       </c>
       <c r="C19">
-        <f ca="1">_xlfn.T.TEST(B2:B11,C2:C11,2,2)</f>
-        <v>0.19662896811676722</v>
-      </c>
-      <c r="D19">
-        <f ca="1">_xlfn.T.TEST(A2:A11,C2:C11,2,2)</f>
-        <v>0.85360310270469841</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <f ca="1">_xlfn.T.TEST(A2:A11,B2:B11,2,3)</f>
-        <v>0.14664818778468452</v>
-      </c>
-      <c r="C20">
-        <f ca="1">_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>0.19691432957251187</v>
-      </c>
-      <c r="D20">
-        <f ca="1">_xlfn.T.TEST(A2:A11,C2:C11,2,3)</f>
-        <v>0.85360315638245943</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B18:D18">
+  <conditionalFormatting sqref="F5:H5">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>

</xml_diff>